<commit_message>
bake the model weights 2
</commit_message>
<xml_diff>
--- a/model/EVAL.xlsx
+++ b/model/EVAL.xlsx
@@ -190,12 +190,18 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFAA95"/>
+        <bgColor rgb="FFFFCC99"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -232,32 +238,52 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -270,6 +296,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFFAA95"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -386,8 +472,8 @@
   </sheetPr>
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Y1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y9" activeCellId="0" sqref="Y9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -726,157 +812,157 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" s="9" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
         <v>73</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="6" t="n">
         <v>224</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="6" t="n">
         <v>165000</v>
       </c>
-      <c r="F5" s="1" t="n">
+      <c r="F5" s="6" t="n">
         <v>64</v>
       </c>
-      <c r="G5" s="1" t="n">
+      <c r="G5" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="H5" s="1" t="n">
+      <c r="H5" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="I5" s="1" t="n">
+      <c r="I5" s="6" t="n">
         <v>7237</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K5" s="1" t="n">
+      <c r="K5" s="6" t="n">
         <v>30</v>
       </c>
-      <c r="L5" s="1" t="n">
+      <c r="L5" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="M5" s="3" t="n">
+      <c r="M5" s="8" t="n">
         <v>0.7643</v>
       </c>
-      <c r="N5" s="3" t="n">
+      <c r="N5" s="8" t="n">
         <v>0.7799</v>
       </c>
-      <c r="O5" s="3" t="n">
+      <c r="O5" s="8" t="n">
         <v>0.0643</v>
       </c>
-      <c r="P5" s="3" t="n">
+      <c r="P5" s="8" t="n">
         <v>0.0632</v>
       </c>
-      <c r="Q5" s="3" t="n">
+      <c r="Q5" s="8" t="n">
         <v>43.4311</v>
       </c>
-      <c r="R5" s="3" t="n">
+      <c r="R5" s="8" t="n">
         <v>44.343</v>
       </c>
-      <c r="S5" s="3" t="n">
+      <c r="S5" s="8" t="n">
         <v>78.74</v>
       </c>
-      <c r="T5" s="3" t="n">
+      <c r="T5" s="8" t="n">
         <v>80.16</v>
       </c>
-      <c r="U5" s="3" t="n">
+      <c r="U5" s="8" t="n">
         <v>87.89</v>
       </c>
-      <c r="V5" s="3" t="n">
+      <c r="V5" s="8" t="n">
         <v>87.76</v>
       </c>
-      <c r="W5" s="1" t="n">
+      <c r="W5" s="6" t="n">
         <v>0.15</v>
       </c>
-      <c r="X5" s="1" t="n">
+      <c r="X5" s="6" t="n">
         <v>0.17</v>
       </c>
-      <c r="Y5" s="1" t="s">
+      <c r="Y5" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+    <row r="6" s="9" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="n">
         <v>74</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="6" t="n">
         <v>224</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="6" t="n">
         <v>197760</v>
       </c>
-      <c r="F6" s="1" t="n">
+      <c r="F6" s="6" t="n">
         <v>32</v>
       </c>
-      <c r="G6" s="1" t="n">
+      <c r="G6" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="H6" s="1" t="n">
+      <c r="H6" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="I6" s="1" t="n">
+      <c r="I6" s="6" t="n">
         <v>7237</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K6" s="1" t="n">
+      <c r="K6" s="6" t="n">
         <v>7.6</v>
       </c>
-      <c r="L6" s="1" t="n">
+      <c r="L6" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="M6" s="3" t="n">
+      <c r="M6" s="8" t="n">
         <v>1.9143</v>
       </c>
-      <c r="N6" s="3" t="n">
+      <c r="N6" s="8" t="n">
         <v>1.9467</v>
       </c>
-      <c r="O6" s="3" t="n">
+      <c r="O6" s="8" t="n">
         <v>0.075</v>
       </c>
-      <c r="P6" s="3" t="n">
+      <c r="P6" s="8" t="n">
         <v>0.0749</v>
       </c>
-      <c r="Q6" s="3" t="n">
+      <c r="Q6" s="8" t="n">
         <v>109.1739</v>
       </c>
-      <c r="R6" s="3" t="n">
+      <c r="R6" s="8" t="n">
         <v>111.0467</v>
       </c>
-      <c r="S6" s="3" t="n">
+      <c r="S6" s="8" t="n">
         <v>74.56</v>
       </c>
-      <c r="T6" s="3" t="n">
+      <c r="T6" s="8" t="n">
         <v>76.37</v>
       </c>
-      <c r="U6" s="3" t="n">
+      <c r="U6" s="8" t="n">
         <v>69.57</v>
       </c>
-      <c r="V6" s="3" t="n">
+      <c r="V6" s="8" t="n">
         <v>69.18</v>
       </c>
-      <c r="W6" s="1" t="n">
+      <c r="W6" s="6" t="n">
         <v>0.17</v>
       </c>
-      <c r="X6" s="1" t="n">
+      <c r="X6" s="6" t="n">
         <v>0.16</v>
       </c>
-      <c r="Y6" s="1" t="s">
+      <c r="Y6" s="6" t="s">
         <v>34</v>
       </c>
     </row>
@@ -891,10 +977,10 @@
         <v>25</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>197760</v>
+        <v>165000</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>32</v>
@@ -1342,162 +1428,162 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+    <row r="13" s="9" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="n">
         <v>77</v>
       </c>
-      <c r="B13" s="1" t="n">
+      <c r="B13" s="6" t="n">
         <v>224</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="1" t="n">
+      <c r="E13" s="6" t="n">
         <f aca="false">1280*256+256*9</f>
         <v>329984</v>
       </c>
-      <c r="F13" s="1" t="n">
+      <c r="F13" s="6" t="n">
         <v>32</v>
       </c>
-      <c r="G13" s="1" t="n">
+      <c r="G13" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="H13" s="1" t="n">
+      <c r="H13" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="I13" s="1" t="n">
+      <c r="I13" s="6" t="n">
         <v>7237</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K13" s="1" t="n">
+      <c r="K13" s="6" t="n">
         <v>33.9</v>
       </c>
-      <c r="L13" s="1" t="n">
+      <c r="L13" s="6" t="n">
         <v>4.9</v>
       </c>
-      <c r="M13" s="1" t="n">
+      <c r="M13" s="6" t="n">
         <v>2.396</v>
       </c>
-      <c r="N13" s="1" t="n">
+      <c r="N13" s="6" t="n">
         <v>2.3865</v>
       </c>
-      <c r="O13" s="1" t="n">
+      <c r="O13" s="6" t="n">
         <v>0.3158</v>
       </c>
-      <c r="P13" s="1" t="n">
+      <c r="P13" s="6" t="n">
         <v>0.3149</v>
       </c>
-      <c r="Q13" s="1" t="n">
+      <c r="Q13" s="6" t="n">
         <v>128.6735</v>
       </c>
-      <c r="R13" s="1" t="n">
+      <c r="R13" s="6" t="n">
         <v>128.1804</v>
       </c>
-      <c r="S13" s="1" t="n">
+      <c r="S13" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="T13" s="1" t="n">
+      <c r="T13" s="6" t="n">
         <v>1.19</v>
       </c>
-      <c r="U13" s="1" t="n">
+      <c r="U13" s="6" t="n">
         <v>64.26</v>
       </c>
-      <c r="V13" s="1" t="n">
+      <c r="V13" s="6" t="n">
         <v>64.39</v>
       </c>
-      <c r="W13" s="1" t="n">
+      <c r="W13" s="6" t="n">
         <v>1.97</v>
       </c>
-      <c r="X13" s="1" t="n">
+      <c r="X13" s="6" t="n">
         <v>2.33</v>
       </c>
-      <c r="Y13" s="1" t="s">
+      <c r="Y13" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+    <row r="14" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="n">
         <v>52</v>
       </c>
-      <c r="B14" s="1" t="n">
+      <c r="B14" s="6" t="n">
         <v>224</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="1" t="n">
+      <c r="E14" s="6" t="n">
         <v>332288</v>
       </c>
-      <c r="F14" s="1" t="n">
+      <c r="F14" s="6" t="n">
         <v>32</v>
       </c>
-      <c r="G14" s="1" t="n">
+      <c r="G14" s="6" t="n">
         <v>30</v>
       </c>
-      <c r="H14" s="1" t="n">
+      <c r="H14" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="I14" s="1" t="n">
+      <c r="I14" s="6" t="n">
         <v>21711</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="J14" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K14" s="1" t="n">
+      <c r="K14" s="6" t="n">
         <v>0.3</v>
       </c>
-      <c r="L14" s="1" t="n">
+      <c r="L14" s="6" t="n">
         <v>2.7</v>
       </c>
-      <c r="M14" s="1" t="n">
+      <c r="M14" s="6" t="n">
         <v>0.8085</v>
       </c>
-      <c r="N14" s="1" t="n">
+      <c r="N14" s="6" t="n">
         <v>0.8367</v>
       </c>
-      <c r="O14" s="1" t="n">
+      <c r="O14" s="6" t="n">
         <v>0.0737</v>
       </c>
-      <c r="P14" s="1" t="n">
+      <c r="P14" s="6" t="n">
         <v>0.0725</v>
       </c>
-      <c r="Q14" s="1" t="n">
+      <c r="Q14" s="6" t="n">
         <v>45.854</v>
       </c>
-      <c r="R14" s="1" t="n">
+      <c r="R14" s="6" t="n">
         <v>47.4849</v>
       </c>
-      <c r="S14" s="1" t="n">
+      <c r="S14" s="6" t="n">
         <v>77.9</v>
       </c>
-      <c r="T14" s="1" t="n">
+      <c r="T14" s="6" t="n">
         <v>78.66</v>
       </c>
-      <c r="U14" s="1" t="n">
+      <c r="U14" s="6" t="n">
         <v>87.26</v>
       </c>
-      <c r="V14" s="1" t="n">
+      <c r="V14" s="6" t="n">
         <v>86.81</v>
       </c>
-      <c r="W14" s="1" t="n">
+      <c r="W14" s="6" t="n">
         <v>0.99</v>
       </c>
-      <c r="X14" s="1" t="n">
+      <c r="X14" s="6" t="n">
         <v>0.99</v>
       </c>
-      <c r="Y14" s="6" t="s">
+      <c r="Y14" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>53</v>
       </c>
@@ -1570,7 +1656,7 @@
       <c r="X15" s="1" t="n">
         <v>0.95</v>
       </c>
-      <c r="Y15" s="6" t="s">
+      <c r="Y15" s="11" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1644,12 +1730,15 @@
       <c r="W16" s="1" t="n">
         <v>0.99</v>
       </c>
-      <c r="X16" s="0" t="n">
+      <c r="X16" s="1" t="n">
         <v>1.1</v>
       </c>
       <c r="Y16" s="1" t="s">
         <v>43</v>
       </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O23" s="1"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>